<commit_message>
working on processing-py version
</commit_message>
<xml_diff>
--- a/sound/List of sounds.xlsx
+++ b/sound/List of sounds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOCUMENTS\Cours ENJMIN\2022-10_Initiation medias interactifs numeriques\moire-project\sound\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C6C7C95-4FC3-4DA6-AB0A-7F76C72BDB5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78468AE0-7D1C-4DD1-982F-7C1E38EBDA2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0BF02138-B187-47F3-8B60-7382D4B2BCF7}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>FOL</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>Clics + autre son quand angle ok</t>
+  </si>
+  <si>
+    <t>TIPS : 3 osc superposés : grave, medium, aigus</t>
+  </si>
+  <si>
+    <t>chacun avec un traitement différent pour donner un son riche</t>
   </si>
 </sst>
 </file>
@@ -117,10 +123,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -437,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB656313-F047-4217-88B3-D01F4AA66F11}">
-  <dimension ref="C1:G8"/>
+  <dimension ref="C1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -450,21 +456,21 @@
     <col min="7" max="7" width="28.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="E1" s="2" t="s">
+    <row r="1" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D5" t="s">
@@ -475,7 +481,7 @@
       </c>
     </row>
     <row r="6" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C6" s="1"/>
+      <c r="C6" s="2"/>
       <c r="D6" t="s">
         <v>3</v>
       </c>
@@ -487,7 +493,7 @@
       </c>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C7" s="1"/>
+      <c r="C7" s="2"/>
       <c r="D7" t="s">
         <v>6</v>
       </c>
@@ -496,7 +502,7 @@
       </c>
     </row>
     <row r="8" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C8" s="1"/>
+      <c r="C8" s="2"/>
       <c r="D8" t="s">
         <v>7</v>
       </c>
@@ -505,6 +511,16 @@
       </c>
       <c r="G8" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>